<commit_message>
Planification Initiale DMA.pdf ajouté
Fin de la planificatin initiale
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>début</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>Préparation présentation</t>
+  </si>
+  <si>
+    <t>lu</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>je</t>
+  </si>
+  <si>
+    <t>ve</t>
   </si>
 </sst>
 </file>
@@ -387,7 +402,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +414,21 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -414,20 +444,20 @@
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F2" s="4">
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G2" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="H2" s="4">
         <v>0</v>
       </c>
       <c r="I2" s="2">
         <f>SUM(D2:H2)</f>
-        <v>0.71875</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="K2" s="3"/>
     </row>
@@ -442,23 +472,23 @@
         <v>2</v>
       </c>
       <c r="D3" s="4">
-        <v>0.21875</v>
+        <v>0.23263888888888887</v>
       </c>
       <c r="E3" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F3" s="4">
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G3" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
       </c>
       <c r="I3" s="2">
         <f>SUM(D3:G3)</f>
-        <v>0.9375</v>
+        <v>0.99652777777777768</v>
       </c>
       <c r="K3" s="3"/>
     </row>
@@ -473,13 +503,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="4">
-        <v>0.21875</v>
+        <v>0.23263888888888887</v>
       </c>
       <c r="E4" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F4" s="4">
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -489,7 +519,7 @@
       </c>
       <c r="I4" s="2">
         <f>SUM(D4:G4)</f>
-        <v>0.65625</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -504,23 +534,23 @@
         <v>4</v>
       </c>
       <c r="D5" s="4">
-        <v>0.21875</v>
+        <v>0.23263888888888887</v>
       </c>
       <c r="E5" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F5" s="4">
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G5" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ref="I5:I7" si="0">SUM(D5:G5)</f>
-        <v>0.9375</v>
+        <v>0.99652777777777768</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -538,10 +568,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F6" s="5">
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G6" s="5">
         <v>0.28125</v>
@@ -550,8 +580,8 @@
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.71875</v>
+        <f>E6</f>
+        <v>0.2986111111111111</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -566,13 +596,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="5">
-        <v>0.21875</v>
+        <v>0.23263888888888887</v>
       </c>
       <c r="E7" s="5">
-        <v>0.28125</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F7" s="5">
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G7" s="5">
         <v>0.28125</v>
@@ -581,8 +611,8 @@
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.9375</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="K7" s="3"/>
     </row>
@@ -598,7 +628,9 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3">
+        <v>90.05</v>
+      </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -627,5 +659,6 @@
     <mergeCell ref="D11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>